<commit_message>
updates to code, and presentation RMD
</commit_message>
<xml_diff>
--- a/cmh/Docu/interim_update/cmhsummary.xlsx
+++ b/cmh/Docu/interim_update/cmhsummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbk/CSRMLW/cmh/Docu/interim_update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\CSRMLW\cmh\Docu\interim_update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E2AB53-1D5B-6A46-8122-357D741F57DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97A6CF0-0B9C-4F19-8719-9C7B79783AFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12320" yWindow="1900" windowWidth="19560" windowHeight="15840" activeTab="2" xr2:uid="{14D2BFBB-038E-4C5F-8875-7F871539408B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14D2BFBB-038E-4C5F-8875-7F871539408B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="59">
   <si>
     <t>Schema</t>
   </si>
@@ -213,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,13 +226,6 @@
       <color rgb="FFCCCCCC"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -335,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,35 +352,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -403,7 +383,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -701,19 +681,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD476B96-7D72-4C73-B6FB-3CDBEA91D454}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -753,7 +733,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -773,7 +753,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -793,7 +773,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -813,7 +793,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -833,7 +813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -853,7 +833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -873,7 +853,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -893,7 +873,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -913,7 +893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -933,7 +913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -953,7 +933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -973,7 +953,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -990,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -1010,7 +990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -1030,7 +1010,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -1050,7 +1030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -1067,7 +1047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -1084,7 +1064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -1101,7 +1081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -1118,7 +1098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1135,7 +1115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -1152,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -1172,7 +1152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -1192,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -1212,7 +1192,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -1232,7 +1212,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -1252,7 +1232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>3</v>
       </c>
@@ -1272,7 +1252,7 @@
         <v>0.30329938000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -1292,7 +1272,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -1312,7 +1292,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -1332,7 +1312,7 @@
         <v>0.30329938000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>3</v>
       </c>
@@ -1352,7 +1332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1372,7 +1352,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -1392,7 +1372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>3</v>
       </c>
@@ -1410,7 +1390,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>3</v>
       </c>
@@ -1430,7 +1410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -1450,7 +1430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>3</v>
       </c>
@@ -1470,7 +1450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -1488,7 +1468,7 @@
       </c>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -1505,7 +1485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>3</v>
       </c>
@@ -1522,7 +1502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>3</v>
       </c>
@@ -1539,7 +1519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -1556,7 +1536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -1573,7 +1553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>9</v>
       </c>
@@ -1593,7 +1573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>9</v>
       </c>
@@ -1613,7 +1593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>9</v>
       </c>
@@ -1633,7 +1613,7 @@
         <v>0.77005224999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>9</v>
       </c>
@@ -1653,7 +1633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>9</v>
       </c>
@@ -1673,7 +1653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>9</v>
       </c>
@@ -1693,7 +1673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>9</v>
       </c>
@@ -1713,7 +1693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>9</v>
       </c>
@@ -1733,7 +1713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>9</v>
       </c>
@@ -1753,7 +1733,7 @@
         <v>0.53298188999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>9</v>
       </c>
@@ -1773,7 +1753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>9</v>
       </c>
@@ -1793,7 +1773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>9</v>
       </c>
@@ -1813,7 +1793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>9</v>
       </c>
@@ -1831,7 +1811,7 @@
       </c>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>9</v>
       </c>
@@ -1851,7 +1831,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>9</v>
       </c>
@@ -1871,7 +1851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>9</v>
       </c>
@@ -1891,7 +1871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>9</v>
       </c>
@@ -1908,7 +1888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>9</v>
       </c>
@@ -1925,7 +1905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>9</v>
       </c>
@@ -1942,7 +1922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>9</v>
       </c>
@@ -1959,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>9</v>
       </c>
@@ -1976,7 +1956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>9</v>
       </c>
@@ -1993,7 +1973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>10</v>
       </c>
@@ -2013,7 +1993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>10</v>
       </c>
@@ -2033,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>10</v>
       </c>
@@ -2053,7 +2033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>10</v>
       </c>
@@ -2073,7 +2053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>10</v>
       </c>
@@ -2093,7 +2073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>10</v>
       </c>
@@ -2113,7 +2093,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>10</v>
       </c>
@@ -2133,7 +2113,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>10</v>
       </c>
@@ -2153,7 +2133,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>10</v>
       </c>
@@ -2173,7 +2153,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>10</v>
       </c>
@@ -2193,7 +2173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>10</v>
       </c>
@@ -2213,7 +2193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>10</v>
       </c>
@@ -2233,7 +2213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>10</v>
       </c>
@@ -2251,7 +2231,7 @@
       </c>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>10</v>
       </c>
@@ -2271,7 +2251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>10</v>
       </c>
@@ -2291,7 +2271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>10</v>
       </c>
@@ -2311,7 +2291,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>10</v>
       </c>
@@ -2328,7 +2308,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>10</v>
       </c>
@@ -2345,7 +2325,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>10</v>
       </c>
@@ -2362,7 +2342,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>10</v>
       </c>
@@ -2379,7 +2359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>10</v>
       </c>
@@ -2396,7 +2376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>10</v>
       </c>
@@ -2413,181 +2393,431 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="15"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="15"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="15"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="15"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="14"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
-    </row>
-    <row r="95" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="16"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="15"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="15"/>
-    </row>
-    <row r="98" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="16"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="14"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="18"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="18"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="18"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="18"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="18"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="18"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="18"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="18"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="15"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="15"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="15"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="15"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="15"/>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>6</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="9">
+        <v>0.13012000000000001</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>6</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="9">
+        <v>1</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>6</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="9">
+        <v>0.71831</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
+        <v>6</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="9">
+        <v>0.13012000000000001</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
+        <v>6</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="9">
+        <v>1</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="9">
+        <v>6</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="9">
+        <v>0.71831</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
+        <v>6</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="12">
+        <v>1.5770999999999999</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
+        <v>6</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="9">
+        <v>4</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="9">
+        <v>6</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" s="9">
+        <v>0.81396999999999997</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
+        <v>6</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="9">
+        <v>6</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>6</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
+        <v>6</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" s="13"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
+        <v>6</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
+        <v>6</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="9">
+        <v>6</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="9">
+        <v>6</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106" s="13"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="9">
+        <v>6</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107" s="10"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="9">
+        <v>6</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F108" s="10"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="9">
+        <v>6</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F109" s="10"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="9">
+        <v>6</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F110" s="10"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="9">
+        <v>6</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F111" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2606,49 +2836,49 @@
       <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2666,13 +2896,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DED4668-0FD0-A04F-B61E-B2CAD8E2211B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9">
         <v>6</v>
       </c>
@@ -2692,7 +2922,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>6</v>
       </c>
@@ -2712,7 +2942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>6</v>
       </c>
@@ -2732,7 +2962,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>6</v>
       </c>
@@ -2752,7 +2982,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>6</v>
       </c>
@@ -2772,7 +3002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>6</v>
       </c>
@@ -2792,7 +3022,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -2812,7 +3042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -2832,7 +3062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2852,7 +3082,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -2872,7 +3102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -2892,7 +3122,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2912,7 +3142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>6</v>
       </c>
@@ -2930,7 +3160,7 @@
       </c>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>6</v>
       </c>
@@ -2950,7 +3180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>6</v>
       </c>
@@ -2970,7 +3200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>6</v>
       </c>
@@ -2990,7 +3220,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>6</v>
       </c>
@@ -3008,7 +3238,7 @@
       </c>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>6</v>
       </c>
@@ -3026,7 +3256,7 @@
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>6</v>
       </c>
@@ -3044,7 +3274,7 @@
       </c>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>6</v>
       </c>
@@ -3062,7 +3292,7 @@
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>6</v>
       </c>
@@ -3080,7 +3310,7 @@
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>6</v>
       </c>
@@ -3100,5 +3330,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;R&amp;1#&amp;"Calibri"&amp;22&amp;KFF8939RESTRICTED</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>